<commit_message>
updated for mar. 20, 2025
</commit_message>
<xml_diff>
--- a/20250227  - Data Science Personal Log.xlsx
+++ b/20250227  - Data Science Personal Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD31D9A-7456-4674-93DA-8CCE244DC763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EC5E01-44EA-45B5-8DD6-46CA15539D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1290" windowWidth="20895" windowHeight="15600" firstSheet="1" activeTab="9" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="24990" yWindow="2325" windowWidth="8595" windowHeight="13935" activeTab="9" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="835">
   <si>
     <t>Movie</t>
   </si>
@@ -1535,12 +1535,6 @@
     <t>3pm</t>
   </si>
   <si>
-    <t>First Round</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Deaner '89</t>
   </si>
   <si>
@@ -1811,9 +1805,6 @@
     <t>Conor</t>
   </si>
   <si>
-    <t>AMW</t>
-  </si>
-  <si>
     <t>not bad, better than I thought. Bonus for cheap</t>
   </si>
   <si>
@@ -2469,6 +2460,99 @@
   </si>
   <si>
     <t>was okay, moderately interesting</t>
+  </si>
+  <si>
+    <t>Home Depot</t>
+  </si>
+  <si>
+    <t>Finance Business Analyst</t>
+  </si>
+  <si>
+    <t>Fairmont</t>
+  </si>
+  <si>
+    <t>Exact Match</t>
+  </si>
+  <si>
+    <t>Presto Recruiting</t>
+  </si>
+  <si>
+    <t>Grunt</t>
+  </si>
+  <si>
+    <t>very good, I liked it. Sad and interesting</t>
+  </si>
+  <si>
+    <t>BUSINESS ANALYST CORPORATE FINANCE (54023)</t>
+  </si>
+  <si>
+    <t>11.22.63</t>
+  </si>
+  <si>
+    <t>hungover</t>
+  </si>
+  <si>
+    <t>last skate of the year got too warm. The ice was very choppy! Fun time though</t>
+  </si>
+  <si>
+    <t>I don’t think its very good but I still order it ocassionally, so they must be doing something right. I see 1600 calories and I get scared</t>
+  </si>
+  <si>
+    <t>A&amp;W</t>
+  </si>
+  <si>
+    <t>Costco</t>
+  </si>
+  <si>
+    <t>Rudys</t>
+  </si>
+  <si>
+    <t>surpringly good</t>
+  </si>
+  <si>
+    <t>Two Point Museum</t>
+  </si>
+  <si>
+    <t>could never finish this game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial Analyst, Marketing Planning &amp; Analysis </t>
+  </si>
+  <si>
+    <t>Freshbooks</t>
+  </si>
+  <si>
+    <t>Bayshore Healthcare</t>
+  </si>
+  <si>
+    <t>Senior Analyst, Business Intelligence</t>
+  </si>
+  <si>
+    <t>StackAdapt</t>
+  </si>
+  <si>
+    <t>Research Analyst (10 month contract)</t>
+  </si>
+  <si>
+    <t>Rakuten</t>
+  </si>
+  <si>
+    <t>Fleetworthy</t>
+  </si>
+  <si>
+    <t>Product Analyst</t>
+  </si>
+  <si>
+    <t>Interview</t>
+  </si>
+  <si>
+    <t>Compunnel</t>
+  </si>
+  <si>
+    <t>Data Analyst, Mapping</t>
+  </si>
+  <si>
+    <t>Lyft</t>
   </si>
 </sst>
 </file>
@@ -4001,10 +4085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5135,13 +5219,13 @@
         <v>5</v>
       </c>
       <c r="K40" t="s">
+        <v>538</v>
+      </c>
+      <c r="L40" t="s">
         <v>540</v>
       </c>
-      <c r="L40" t="s">
-        <v>542</v>
-      </c>
       <c r="M40" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -5173,7 +5257,7 @@
         <v>458</v>
       </c>
       <c r="M41" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -5181,7 +5265,7 @@
         <v>45665</v>
       </c>
       <c r="B42" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C42">
         <v>8.1</v>
@@ -5202,7 +5286,7 @@
         <v>6</v>
       </c>
       <c r="K42" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -5231,7 +5315,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -5263,7 +5347,7 @@
         <v>458</v>
       </c>
       <c r="M44" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -5292,7 +5376,7 @@
         <v>3</v>
       </c>
       <c r="M45" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -5321,7 +5405,7 @@
         <v>5</v>
       </c>
       <c r="M46" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -5350,7 +5434,7 @@
         <v>3</v>
       </c>
       <c r="M47" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -5379,7 +5463,7 @@
         <v>5</v>
       </c>
       <c r="M48" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -5402,7 +5486,7 @@
         <v>1</v>
       </c>
       <c r="M49" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -5425,7 +5509,7 @@
         <v>2</v>
       </c>
       <c r="M50" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -5448,10 +5532,10 @@
         <v>1</v>
       </c>
       <c r="K51" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="M51" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -5480,13 +5564,13 @@
         <v>2</v>
       </c>
       <c r="K52" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="L52" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="M52" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -5515,10 +5599,10 @@
         <v>1</v>
       </c>
       <c r="K53" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="M53" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -5547,10 +5631,10 @@
         <v>4</v>
       </c>
       <c r="K54" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="M54" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -5579,7 +5663,7 @@
         <v>5</v>
       </c>
       <c r="M55" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -5611,13 +5695,13 @@
         <v>6</v>
       </c>
       <c r="J56" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="K56" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="M56" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -5646,13 +5730,13 @@
         <v>4</v>
       </c>
       <c r="K57" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="L57" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="M57" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -5681,13 +5765,13 @@
         <v>6</v>
       </c>
       <c r="K58" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="L58" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="M58" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -5727,7 +5811,7 @@
         <v>45709</v>
       </c>
       <c r="B60" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C60">
         <v>7.8</v>
@@ -5748,10 +5832,10 @@
         <v>2</v>
       </c>
       <c r="K60" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="M60" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -5759,7 +5843,7 @@
         <v>45710</v>
       </c>
       <c r="B61" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C61">
         <v>7.5</v>
@@ -5785,7 +5869,7 @@
         <v>45711</v>
       </c>
       <c r="B62" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C62">
         <v>6.6</v>
@@ -5806,7 +5890,7 @@
         <v>3</v>
       </c>
       <c r="M62" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -5835,12 +5919,12 @@
         <v>5</v>
       </c>
       <c r="M63" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>45715</v>
+        <v>45714</v>
       </c>
       <c r="B64" t="s">
         <v>224</v>
@@ -5864,10 +5948,63 @@
         <v>2</v>
       </c>
       <c r="K64" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="M64" t="s">
-        <v>794</v>
+        <v>791</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>45721</v>
+      </c>
+      <c r="B65" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>45723</v>
+      </c>
+      <c r="B66" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>45725</v>
+      </c>
+      <c r="B67" t="s">
+        <v>489</v>
+      </c>
+      <c r="C67">
+        <v>7.3</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>3</v>
+      </c>
+      <c r="L67" t="s">
+        <v>813</v>
+      </c>
+      <c r="M67" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>45726</v>
       </c>
     </row>
   </sheetData>
@@ -5877,10 +6014,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="B80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5915,13 +6052,13 @@
         <v>402</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="H1" t="s">
         <v>390</v>
       </c>
       <c r="J1" t="s">
-        <v>495</v>
+        <v>831</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5949,9 +6086,6 @@
       </c>
       <c r="I2" t="s">
         <v>391</v>
-      </c>
-      <c r="J2" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6183,7 +6317,7 @@
         <v>45623</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>446</v>
@@ -6247,16 +6381,16 @@
         <v>45645</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6276,7 +6410,7 @@
         <v>407</v>
       </c>
       <c r="H18" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I18" t="s">
         <v>391</v>
@@ -6287,10 +6421,10 @@
         <v>45653</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
@@ -6304,16 +6438,16 @@
         <v>45661</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="7" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -6321,10 +6455,10 @@
         <v>45661</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -6338,16 +6472,16 @@
         <v>45662</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="7" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6355,16 +6489,16 @@
         <v>45663</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="7" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6372,16 +6506,16 @@
         <v>45663</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="7" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -6389,16 +6523,16 @@
         <v>45664</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="7" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -6406,16 +6540,16 @@
         <v>45665</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="7" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -6423,16 +6557,16 @@
         <v>45665</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="7" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -6440,16 +6574,16 @@
         <v>45667</v>
       </c>
       <c r="B28" t="s">
+        <v>576</v>
+      </c>
+      <c r="C28" t="s">
+        <v>577</v>
+      </c>
+      <c r="F28" t="s">
+        <v>581</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>578</v>
-      </c>
-      <c r="C28" t="s">
-        <v>579</v>
-      </c>
-      <c r="F28" t="s">
-        <v>583</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -6457,16 +6591,16 @@
         <v>45667</v>
       </c>
       <c r="B29" t="s">
+        <v>580</v>
+      </c>
+      <c r="C29" t="s">
+        <v>579</v>
+      </c>
+      <c r="F29" t="s">
         <v>582</v>
       </c>
-      <c r="C29" t="s">
-        <v>581</v>
-      </c>
-      <c r="F29" t="s">
-        <v>584</v>
-      </c>
       <c r="G29" s="13" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -6474,13 +6608,13 @@
         <v>45669</v>
       </c>
       <c r="B30" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C30" t="s">
         <v>393</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -6491,10 +6625,10 @@
         <v>423</v>
       </c>
       <c r="C31" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F31" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>408</v>
@@ -6505,13 +6639,13 @@
         <v>45670</v>
       </c>
       <c r="B32" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C32" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -6519,16 +6653,16 @@
         <v>45671</v>
       </c>
       <c r="B33" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C33" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F33" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -6536,13 +6670,13 @@
         <v>45671</v>
       </c>
       <c r="B34" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C34" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -6550,7 +6684,7 @@
         <v>45671</v>
       </c>
       <c r="B35" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C35" t="s">
         <v>393</v>
@@ -6561,19 +6695,19 @@
         <v>45671</v>
       </c>
       <c r="B36" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C36" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E36" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="F36" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -6581,10 +6715,10 @@
         <v>45671</v>
       </c>
       <c r="B37" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C37" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6592,13 +6726,13 @@
         <v>45671</v>
       </c>
       <c r="B38" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C38" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6606,13 +6740,13 @@
         <v>45671</v>
       </c>
       <c r="B39" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C39" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6620,16 +6754,16 @@
         <v>45671</v>
       </c>
       <c r="B40" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C40" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="F40" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G40" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6637,16 +6771,16 @@
         <v>45681</v>
       </c>
       <c r="B41" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C41" t="s">
         <v>421</v>
       </c>
       <c r="F41" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="G41" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6654,16 +6788,16 @@
         <v>45684</v>
       </c>
       <c r="B42" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C42" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="F42" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="G42" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6671,16 +6805,16 @@
         <v>45685</v>
       </c>
       <c r="B43" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C43" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="F43" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="G43" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -6688,13 +6822,13 @@
         <v>45686</v>
       </c>
       <c r="B44" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C44" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="G44" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -6702,13 +6836,13 @@
         <v>45687</v>
       </c>
       <c r="B45" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C45" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="G45" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -6716,13 +6850,13 @@
         <v>45688</v>
       </c>
       <c r="B46" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="C46" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="G46" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -6730,13 +6864,13 @@
         <v>45688</v>
       </c>
       <c r="B47" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C47" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="G47" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -6744,13 +6878,13 @@
         <v>45690</v>
       </c>
       <c r="B48" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="C48" t="s">
         <v>421</v>
       </c>
       <c r="G48" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -6758,13 +6892,13 @@
         <v>45692</v>
       </c>
       <c r="B49" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C49" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="G49" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -6772,13 +6906,13 @@
         <v>45692</v>
       </c>
       <c r="B50" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="C50" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="G50" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -6786,13 +6920,13 @@
         <v>45694</v>
       </c>
       <c r="B51" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="C51" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="G51" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -6800,13 +6934,13 @@
         <v>45699</v>
       </c>
       <c r="B52" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="C52" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="G52" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -6814,16 +6948,16 @@
         <v>45699</v>
       </c>
       <c r="B53" t="s">
+        <v>717</v>
+      </c>
+      <c r="C53" t="s">
+        <v>719</v>
+      </c>
+      <c r="E53" t="s">
         <v>720</v>
       </c>
-      <c r="C53" t="s">
-        <v>722</v>
-      </c>
-      <c r="E53" t="s">
-        <v>723</v>
-      </c>
       <c r="G53" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -6834,10 +6968,10 @@
         <v>451</v>
       </c>
       <c r="C54" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="G54" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -6845,13 +6979,13 @@
         <v>45700</v>
       </c>
       <c r="B55" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C55" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="G55" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -6859,16 +6993,16 @@
         <v>45700</v>
       </c>
       <c r="B56" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C56" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="F56" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="G56" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -6876,16 +7010,16 @@
         <v>45701</v>
       </c>
       <c r="B57" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C57" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="E57" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="G57" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -6893,13 +7027,13 @@
         <v>45702</v>
       </c>
       <c r="B58" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C58" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="G58" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -6907,13 +7041,13 @@
         <v>45702</v>
       </c>
       <c r="B59" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C59" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="G59" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -6921,13 +7055,13 @@
         <v>45702</v>
       </c>
       <c r="B60" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C60" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="G60" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -6935,13 +7069,13 @@
         <v>45706</v>
       </c>
       <c r="B61" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="C61" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="G61" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -6949,13 +7083,13 @@
         <v>45706</v>
       </c>
       <c r="B62" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="C62" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="G62" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -6966,10 +7100,10 @@
         <v>404</v>
       </c>
       <c r="C63" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="G63" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -6977,16 +7111,16 @@
         <v>45706</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C64" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="G64" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H64" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="I64" t="s">
         <v>391</v>
@@ -6997,13 +7131,13 @@
         <v>45706</v>
       </c>
       <c r="B65" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="C65" t="s">
         <v>393</v>
       </c>
       <c r="G65" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -7011,16 +7145,16 @@
         <v>45712</v>
       </c>
       <c r="B66" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C66" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="F66" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="G66" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -7028,16 +7162,16 @@
         <v>45712</v>
       </c>
       <c r="B67" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="C67" t="s">
         <v>404</v>
       </c>
       <c r="F67" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="G67" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -7045,16 +7179,16 @@
         <v>45712</v>
       </c>
       <c r="B68" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="C68" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="F68" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="G68" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -7062,16 +7196,16 @@
         <v>45712</v>
       </c>
       <c r="B69" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C69" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="F69" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="G69" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -7079,16 +7213,16 @@
         <v>45712</v>
       </c>
       <c r="B70" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C70" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="F70" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="G70" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -7099,10 +7233,10 @@
         <v>404</v>
       </c>
       <c r="C71" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="G71" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -7110,13 +7244,13 @@
         <v>45713</v>
       </c>
       <c r="B72" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="C72" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="G72" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -7127,10 +7261,10 @@
         <v>428</v>
       </c>
       <c r="C73" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="G73" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -7138,13 +7272,13 @@
         <v>45714</v>
       </c>
       <c r="B74" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C74" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="G74" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -7155,10 +7289,10 @@
         <v>404</v>
       </c>
       <c r="C75" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G75" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -7166,13 +7300,13 @@
         <v>45714</v>
       </c>
       <c r="B76" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C76" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="G76" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -7180,13 +7314,13 @@
         <v>45715</v>
       </c>
       <c r="B77" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="C77" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="G77" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -7194,13 +7328,13 @@
         <v>45715</v>
       </c>
       <c r="B78" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="C78" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="G78" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -7211,10 +7345,186 @@
         <v>404</v>
       </c>
       <c r="C79" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="G79" t="s">
-        <v>563</v>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B80" t="s">
+        <v>404</v>
+      </c>
+      <c r="C80" t="s">
+        <v>804</v>
+      </c>
+      <c r="G80" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B81" t="s">
+        <v>805</v>
+      </c>
+      <c r="C81" t="s">
+        <v>806</v>
+      </c>
+      <c r="G81" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B82" t="s">
+        <v>404</v>
+      </c>
+      <c r="C82" t="s">
+        <v>807</v>
+      </c>
+      <c r="G82" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>45716</v>
+      </c>
+      <c r="B83" t="s">
+        <v>404</v>
+      </c>
+      <c r="C83" t="s">
+        <v>808</v>
+      </c>
+      <c r="G83" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>45721</v>
+      </c>
+      <c r="B84" t="s">
+        <v>811</v>
+      </c>
+      <c r="C84" t="s">
+        <v>421</v>
+      </c>
+      <c r="G84" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B85" t="s">
+        <v>822</v>
+      </c>
+      <c r="C85" t="s">
+        <v>823</v>
+      </c>
+      <c r="G85" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B86" t="s">
+        <v>451</v>
+      </c>
+      <c r="C86" t="s">
+        <v>824</v>
+      </c>
+      <c r="G86" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B87" t="s">
+        <v>825</v>
+      </c>
+      <c r="C87" t="s">
+        <v>824</v>
+      </c>
+      <c r="G87" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B88" t="s">
+        <v>404</v>
+      </c>
+      <c r="C88" t="s">
+        <v>826</v>
+      </c>
+      <c r="G88" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B89" t="s">
+        <v>830</v>
+      </c>
+      <c r="C89" t="s">
+        <v>829</v>
+      </c>
+      <c r="G89" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B90" t="s">
+        <v>827</v>
+      </c>
+      <c r="C90" t="s">
+        <v>828</v>
+      </c>
+      <c r="G90" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B91" t="s">
+        <v>404</v>
+      </c>
+      <c r="C91" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B92" t="s">
+        <v>833</v>
+      </c>
+      <c r="C92" t="s">
+        <v>834</v>
       </c>
     </row>
   </sheetData>
@@ -7241,7 +7551,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -7253,16 +7563,16 @@
         <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="G1" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="I1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J1" t="s">
         <v>18</v>
@@ -7279,13 +7589,13 @@
         <v>7.6</v>
       </c>
       <c r="D2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E2" t="s">
         <v>349</v>
       </c>
       <c r="F2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G2" s="15">
         <v>0.9</v>
@@ -7294,13 +7604,13 @@
         <v>0.4</v>
       </c>
       <c r="I2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="J2">
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -7308,19 +7618,19 @@
         <v>45671</v>
       </c>
       <c r="B3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C3">
         <v>7.7</v>
       </c>
       <c r="D3" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="G3" s="15">
         <v>0.05</v>
@@ -7329,13 +7639,13 @@
         <v>0.99</v>
       </c>
       <c r="I3" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J3">
         <v>75</v>
       </c>
       <c r="K3" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -7688,10 +7998,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7715,7 +8025,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -7724,7 +8034,7 @@
         <v>86</v>
       </c>
       <c r="H1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -8218,7 +8528,7 @@
         <v>45517</v>
       </c>
       <c r="B23" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C23">
         <v>8.1999999999999993</v>
@@ -8233,7 +8543,7 @@
         <v>91</v>
       </c>
       <c r="I23" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -8624,7 +8934,7 @@
         <v>318</v>
       </c>
       <c r="I40" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -8770,13 +9080,13 @@
         <v>45638</v>
       </c>
       <c r="B47" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C47">
         <v>8.9</v>
       </c>
       <c r="D47" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F47" t="s">
         <v>49</v>
@@ -8785,7 +9095,7 @@
         <v>300</v>
       </c>
       <c r="I47" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -8793,7 +9103,7 @@
         <v>45640</v>
       </c>
       <c r="B48" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C48">
         <v>7</v>
@@ -8808,7 +9118,7 @@
         <v>300</v>
       </c>
       <c r="I48" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -8816,7 +9126,7 @@
         <v>45641</v>
       </c>
       <c r="B49" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C49">
         <v>8.6</v>
@@ -8831,7 +9141,7 @@
         <v>300</v>
       </c>
       <c r="I49" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -8839,13 +9149,13 @@
         <v>45643</v>
       </c>
       <c r="B50" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C50">
         <v>7.7</v>
       </c>
       <c r="D50" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F50" t="s">
         <v>49</v>
@@ -8854,7 +9164,7 @@
         <v>91</v>
       </c>
       <c r="I50" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -8862,7 +9172,7 @@
         <v>45647</v>
       </c>
       <c r="B51" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C51">
         <v>7.8</v>
@@ -8877,7 +9187,7 @@
         <v>91</v>
       </c>
       <c r="I51" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -8885,7 +9195,7 @@
         <v>45648</v>
       </c>
       <c r="B52" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C52">
         <v>6.1</v>
@@ -8900,7 +9210,7 @@
         <v>91</v>
       </c>
       <c r="I52" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -8908,13 +9218,13 @@
         <v>45653</v>
       </c>
       <c r="B53" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C53">
         <v>7.8</v>
       </c>
       <c r="D53" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F53" t="s">
         <v>49</v>
@@ -8923,7 +9233,7 @@
         <v>87</v>
       </c>
       <c r="I53" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -8931,7 +9241,7 @@
         <v>45660</v>
       </c>
       <c r="B54" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C54">
         <v>8.9</v>
@@ -8946,7 +9256,7 @@
         <v>87</v>
       </c>
       <c r="I54" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -8954,7 +9264,7 @@
         <v>45661</v>
       </c>
       <c r="B55" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C55">
         <v>8.1</v>
@@ -8969,7 +9279,7 @@
         <v>300</v>
       </c>
       <c r="I55" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -8977,13 +9287,13 @@
         <v>45666</v>
       </c>
       <c r="B56" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C56">
         <v>7.1</v>
       </c>
       <c r="D56" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E56">
         <v>2023</v>
@@ -8995,7 +9305,7 @@
         <v>300</v>
       </c>
       <c r="I56" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -9003,7 +9313,7 @@
         <v>45667</v>
       </c>
       <c r="B57" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C57">
         <v>7.3</v>
@@ -9021,7 +9331,7 @@
         <v>300</v>
       </c>
       <c r="I57" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -9029,13 +9339,13 @@
         <v>45668</v>
       </c>
       <c r="B58" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C58">
         <v>9.3000000000000007</v>
       </c>
       <c r="D58" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E58">
         <v>2024</v>
@@ -9047,7 +9357,7 @@
         <v>87</v>
       </c>
       <c r="I58" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -9055,7 +9365,7 @@
         <v>45669</v>
       </c>
       <c r="B59" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C59">
         <v>7.1</v>
@@ -9073,10 +9383,10 @@
         <v>442</v>
       </c>
       <c r="H59" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="I59" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -9084,13 +9394,13 @@
         <v>45671</v>
       </c>
       <c r="B60" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C60">
         <v>7.2</v>
       </c>
       <c r="D60" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E60">
         <v>1998</v>
@@ -9102,13 +9412,13 @@
         <v>231</v>
       </c>
       <c r="I60" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
@@ -9122,7 +9432,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -9136,7 +9446,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
@@ -9153,7 +9463,7 @@
         <v>45674</v>
       </c>
       <c r="B64" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C64">
         <v>6.8</v>
@@ -9168,7 +9478,7 @@
         <v>231</v>
       </c>
       <c r="I64" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -9176,7 +9486,7 @@
         <v>45673</v>
       </c>
       <c r="B65" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C65">
         <v>8.1</v>
@@ -9191,17 +9501,17 @@
         <v>231</v>
       </c>
       <c r="I65" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -9209,13 +9519,13 @@
         <v>45674</v>
       </c>
       <c r="B68" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C68">
         <v>7.2</v>
       </c>
       <c r="D68" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E68">
         <v>2025</v>
@@ -9227,7 +9537,7 @@
         <v>231</v>
       </c>
       <c r="I68" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -9235,7 +9545,7 @@
         <v>45670</v>
       </c>
       <c r="B69" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C69">
         <v>7.6</v>
@@ -9250,7 +9560,7 @@
         <v>231</v>
       </c>
       <c r="I69" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -9258,13 +9568,13 @@
         <v>45677</v>
       </c>
       <c r="B70" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C70">
         <v>6.8</v>
       </c>
       <c r="D70" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="E70">
         <v>2009</v>
@@ -9276,7 +9586,7 @@
         <v>91</v>
       </c>
       <c r="I70" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -9284,22 +9594,22 @@
         <v>45677</v>
       </c>
       <c r="B71" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C71">
         <v>7.7</v>
       </c>
       <c r="D71" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="E71">
         <v>1992</v>
       </c>
       <c r="G71" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="I71" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -9307,13 +9617,13 @@
         <v>45677</v>
       </c>
       <c r="B72" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C72">
         <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="E72">
         <v>2024</v>
@@ -9325,7 +9635,7 @@
         <v>231</v>
       </c>
       <c r="I72" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -9333,7 +9643,7 @@
         <v>45678</v>
       </c>
       <c r="B73" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C73">
         <v>6.7</v>
@@ -9351,7 +9661,7 @@
         <v>231</v>
       </c>
       <c r="I73" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -9359,7 +9669,7 @@
         <v>45678</v>
       </c>
       <c r="B74" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C74">
         <v>6.8</v>
@@ -9377,7 +9687,7 @@
         <v>231</v>
       </c>
       <c r="I74" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -9385,7 +9695,7 @@
         <v>45685</v>
       </c>
       <c r="B75" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C75">
         <v>7.7</v>
@@ -9400,7 +9710,7 @@
         <v>442</v>
       </c>
       <c r="I75" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -9427,7 +9737,7 @@
         <v>231</v>
       </c>
       <c r="I76" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -9435,7 +9745,7 @@
         <v>45687</v>
       </c>
       <c r="B77" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C77">
         <v>7.2</v>
@@ -9453,7 +9763,7 @@
         <v>231</v>
       </c>
       <c r="I77" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -9461,7 +9771,7 @@
         <v>45691</v>
       </c>
       <c r="B78" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="C78">
         <v>7.4</v>
@@ -9484,7 +9794,7 @@
         <v>45692</v>
       </c>
       <c r="B79" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C79">
         <v>7.6</v>
@@ -9499,7 +9809,7 @@
         <v>442</v>
       </c>
       <c r="I79" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -9507,7 +9817,7 @@
         <v>45700</v>
       </c>
       <c r="B80" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C80">
         <v>6.7</v>
@@ -9522,7 +9832,7 @@
         <v>231</v>
       </c>
       <c r="I80" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -9530,13 +9840,13 @@
         <v>45701</v>
       </c>
       <c r="B81" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C81">
         <v>7.4</v>
       </c>
       <c r="D81" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E81">
         <v>2024</v>
@@ -9548,7 +9858,7 @@
         <v>91</v>
       </c>
       <c r="I81" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -9556,7 +9866,7 @@
         <v>45703</v>
       </c>
       <c r="B82" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="C82">
         <v>5.8</v>
@@ -9573,7 +9883,7 @@
         <v>45703</v>
       </c>
       <c r="B83" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="C83">
         <v>6.3</v>
@@ -9596,7 +9906,7 @@
         <v>45704</v>
       </c>
       <c r="B84" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="C84">
         <v>6.2</v>
@@ -9614,7 +9924,7 @@
         <v>231</v>
       </c>
       <c r="I84" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -9622,13 +9932,13 @@
         <v>45704</v>
       </c>
       <c r="B85" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C85">
         <v>7.8</v>
       </c>
       <c r="D85" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E85">
         <v>2025</v>
@@ -9640,7 +9950,7 @@
         <v>231</v>
       </c>
       <c r="I85" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -9648,7 +9958,7 @@
         <v>45705</v>
       </c>
       <c r="B86" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="C86">
         <v>8</v>
@@ -9674,13 +9984,13 @@
         <v>45715</v>
       </c>
       <c r="B87" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="C87">
         <v>6.5</v>
       </c>
       <c r="D87" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="E87">
         <v>2025</v>
@@ -9692,7 +10002,7 @@
         <v>231</v>
       </c>
       <c r="I87" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -9700,7 +10010,7 @@
         <v>45715</v>
       </c>
       <c r="B88" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="C88">
         <v>7.1</v>
@@ -9718,7 +10028,33 @@
         <v>231</v>
       </c>
       <c r="I88" t="s">
-        <v>806</v>
+        <v>803</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>45721</v>
+      </c>
+      <c r="B89" t="s">
+        <v>809</v>
+      </c>
+      <c r="C89">
+        <v>7.9</v>
+      </c>
+      <c r="D89" t="s">
+        <v>120</v>
+      </c>
+      <c r="E89">
+        <v>2025</v>
+      </c>
+      <c r="F89" t="s">
+        <v>49</v>
+      </c>
+      <c r="G89" t="s">
+        <v>654</v>
+      </c>
+      <c r="I89" t="s">
+        <v>810</v>
       </c>
     </row>
   </sheetData>
@@ -9728,10 +10064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10100,7 +10436,7 @@
         <v>438</v>
       </c>
       <c r="G14" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -10184,7 +10520,7 @@
         <v>45647</v>
       </c>
       <c r="B20" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -10202,7 +10538,7 @@
         <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -10210,7 +10546,7 @@
         <v>45670</v>
       </c>
       <c r="B21" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -10228,7 +10564,7 @@
         <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -10236,7 +10572,7 @@
         <v>45663</v>
       </c>
       <c r="B22" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -10254,7 +10590,7 @@
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -10262,7 +10598,7 @@
         <v>45665</v>
       </c>
       <c r="B23" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -10276,7 +10612,7 @@
         <v>45680</v>
       </c>
       <c r="B24" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -10294,12 +10630,12 @@
         <v>11</v>
       </c>
       <c r="H24" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -10313,7 +10649,7 @@
         <v>45715</v>
       </c>
       <c r="B26" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -10321,7 +10657,7 @@
         <v>45699</v>
       </c>
       <c r="B27" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -10339,7 +10675,7 @@
         <v>11</v>
       </c>
       <c r="H27" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -10347,7 +10683,7 @@
         <v>45702</v>
       </c>
       <c r="B28" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -10365,12 +10701,12 @@
         <v>11</v>
       </c>
       <c r="H28" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -10382,12 +10718,12 @@
         <v>11</v>
       </c>
       <c r="H29" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -10395,7 +10731,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="C31">
         <v>11</v>
@@ -10406,7 +10742,7 @@
         <v>45714</v>
       </c>
       <c r="B32" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -10424,12 +10760,17 @@
         <v>11</v>
       </c>
       <c r="H32" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>796</v>
+        <v>793</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>812</v>
       </c>
     </row>
   </sheetData>
@@ -10439,10 +10780,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10796,7 +11137,7 @@
         <v>45592</v>
       </c>
       <c r="B14" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C14">
         <v>5.6</v>
@@ -10970,7 +11311,7 @@
         <v>96</v>
       </c>
       <c r="H20" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -10996,7 +11337,7 @@
         <v>96</v>
       </c>
       <c r="H21" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -11004,7 +11345,7 @@
         <v>45667</v>
       </c>
       <c r="B22" t="s">
-        <v>587</v>
+        <v>816</v>
       </c>
       <c r="C22">
         <v>6.9</v>
@@ -11022,7 +11363,7 @@
         <v>96</v>
       </c>
       <c r="H22" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -11030,7 +11371,7 @@
         <v>45680</v>
       </c>
       <c r="B23" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C23">
         <v>6.9</v>
@@ -11048,7 +11389,7 @@
         <v>96</v>
       </c>
       <c r="H23" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -11056,7 +11397,7 @@
         <v>45690</v>
       </c>
       <c r="B24" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C24">
         <v>6.8</v>
@@ -11071,10 +11412,10 @@
         <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="H24" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -11094,13 +11435,65 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="G25" t="s">
         <v>96</v>
       </c>
       <c r="H25" t="s">
-        <v>716</v>
+        <v>713</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>45719</v>
+      </c>
+      <c r="B26" t="s">
+        <v>818</v>
+      </c>
+      <c r="C26">
+        <v>7.9</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B27" t="s">
+        <v>817</v>
+      </c>
+      <c r="C27">
+        <v>6.6</v>
+      </c>
+      <c r="D27">
+        <v>6.75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" t="s">
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -11110,10 +11503,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CAB6AD-E088-49BC-A679-AC7F288052E6}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11337,22 +11730,46 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>592</v>
+        <v>589</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45656</v>
+      </c>
+      <c r="D12">
+        <v>2025</v>
+      </c>
+      <c r="E12">
+        <v>8.4</v>
+      </c>
+      <c r="F12">
+        <v>8.6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>734</v>
+        <v>731</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45687</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="B15" s="2">
         <v>45705</v>
@@ -11371,6 +11788,11 @@
       </c>
       <c r="H15" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -11383,7 +11805,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11532,7 +11954,7 @@
         <v>457</v>
       </c>
       <c r="C8" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D8" t="s">
         <v>135</v>
@@ -11544,7 +11966,7 @@
         <v>8.5</v>
       </c>
       <c r="G8" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -11567,10 +11989,10 @@
         <v>45323</v>
       </c>
       <c r="B10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C10" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D10" t="s">
         <v>135</v>
@@ -11582,15 +12004,15 @@
         <v>9.6</v>
       </c>
       <c r="G10" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -12031,7 +12453,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C9">
         <v>93</v>
@@ -12042,7 +12464,7 @@
         <v>45670</v>
       </c>
       <c r="B10" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -12051,7 +12473,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -12153,7 +12575,7 @@
         <v>45641</v>
       </c>
       <c r="B4" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>